<commit_message>
codigo de graficos y cambio algunas cosas de informe
</commit_message>
<xml_diff>
--- a/Trabajo práctico 3/Bases limpias/Población tipo.xlsx
+++ b/Trabajo práctico 3/Bases limpias/Población tipo.xlsx
@@ -412,7 +412,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0945207547255415</v>
+        <v>0.945207547255415</v>
       </c>
     </row>
     <row r="4">
@@ -426,7 +426,7 @@
         <v>40</v>
       </c>
       <c r="D4" t="n">
-        <v>0.422977938105215</v>
+        <v>4.22977938105215</v>
       </c>
     </row>
     <row r="5">
@@ -440,7 +440,7 @@
         <v>100</v>
       </c>
       <c r="D5" t="n">
-        <v>1.4479566725029</v>
+        <v>14.479566725029</v>
       </c>
     </row>
     <row r="6">
@@ -454,7 +454,7 @@
         <v>175</v>
       </c>
       <c r="D6" t="n">
-        <v>3.62914380824517</v>
+        <v>36.2914380824517</v>
       </c>
     </row>
     <row r="7">
@@ -468,7 +468,7 @@
         <v>155</v>
       </c>
       <c r="D7" t="n">
-        <v>7.17159972479564</v>
+        <v>71.7159972479564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>